<commit_message>
Pre-deploy verification: all checks passed, ready for Railway
</commit_message>
<xml_diff>
--- a/maestro_completo.xlsx
+++ b/maestro_completo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
   <si>
     <t>id</t>
   </si>
@@ -45,7 +45,7 @@
     <t>activo</t>
   </si>
   <si>
-    <t>Precio novillo hacienda (INAC) – USD/4ta balanza</t>
+    <t>link</t>
   </si>
   <si>
     <t>P</t>
@@ -60,7 +60,7 @@
     <t>USD/kg</t>
   </si>
   <si>
-    <t>Exportación leche en polvo entera – INALE</t>
+    <t>Carne</t>
   </si>
   <si>
     <t>INALE – Exportación leche en polvo entera</t>
@@ -72,88 +72,160 @@
     <t>Lácteos</t>
   </si>
   <si>
-    <t>Exportación queso – INALE</t>
-  </si>
-  <si>
     <t>INALE – Exportación queso</t>
   </si>
   <si>
-    <t>Precio al productor de leche – INALE</t>
-  </si>
-  <si>
     <t>INALE – Precio leche en tambo y composición</t>
   </si>
   <si>
     <t>UYU/litro</t>
   </si>
   <si>
+    <t>W</t>
+  </si>
+  <si>
     <t>Tipo de cambio USD/UYU (promedio compra-venta)</t>
   </si>
   <si>
+    <t>INE</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
     <t>UYU por USD</t>
   </si>
   <si>
+    <t>Macro</t>
+  </si>
+  <si>
     <t>Tipo de cambio EUR/UYU (promedio compra-venta)</t>
   </si>
   <si>
     <t>UYU por EUR</t>
   </si>
   <si>
-    <t>Precio soja - Banco Mundial (CMO Historical Data)</t>
-  </si>
-  <si>
     <t>WorldBank_CMO</t>
   </si>
   <si>
-    <t>Precio arroz - Banco Mundial (CMO Historical Data)</t>
-  </si>
-  <si>
-    <t>Precio trigo - Banco Mundial (CMO Historical Data)</t>
-  </si>
-  <si>
-    <t>Precio exportacion carne (INAC)</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Carne</t>
-  </si>
-  <si>
     <t>Granos</t>
   </si>
   <si>
-    <t>mercado</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>IPC</t>
   </si>
   <si>
-    <t>INE</t>
-  </si>
-  <si>
     <t>Indice</t>
   </si>
   <si>
-    <t>Macro</t>
-  </si>
-  <si>
-    <t>Celulosa</t>
-  </si>
-  <si>
-    <t>INSEE</t>
-  </si>
-  <si>
-    <t>Madera</t>
+    <t>INSEE - serie 010600341 (Producer Price Index - Pulp)</t>
+  </si>
+  <si>
+    <t>Productos forestales</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU513210513210</t>
+  </si>
+  <si>
+    <t>Ingeniería</t>
+  </si>
+  <si>
+    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU541330541330</t>
+  </si>
+  <si>
+    <t>Arquitectura</t>
+  </si>
+  <si>
+    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU541310541310</t>
+  </si>
+  <si>
+    <t>Contabilidad (CPA)</t>
+  </si>
+  <si>
+    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU541211541211</t>
+  </si>
+  <si>
+    <t>Bookkeeping / payroll</t>
+  </si>
+  <si>
+    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU541211541211A</t>
+  </si>
+  <si>
+    <t>moneda</t>
+  </si>
+  <si>
+    <t>usd</t>
+  </si>
+  <si>
+    <t>eur</t>
+  </si>
+  <si>
+    <t>Precio hacienda</t>
+  </si>
+  <si>
+    <t>Leche en polvo</t>
+  </si>
+  <si>
+    <t>Precio leche productor</t>
+  </si>
+  <si>
+    <t>Precio carne export</t>
+  </si>
+  <si>
+    <t>Soja</t>
+  </si>
+  <si>
+    <t>Arroz</t>
+  </si>
+  <si>
+    <t>Trigo</t>
+  </si>
+  <si>
+    <t>Celulosa -indice-</t>
+  </si>
+  <si>
+    <t>Servicios no tradicionales - sin software</t>
+  </si>
+  <si>
+    <t>Queso</t>
+  </si>
+  <si>
+    <t>nominal_real</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Salario real</t>
+  </si>
+  <si>
+    <t>uyu</t>
+  </si>
+  <si>
+    <t>Gasoil</t>
+  </si>
+  <si>
+    <t>ANCAP</t>
+  </si>
+  <si>
+    <t>$ por Litro</t>
+  </si>
+  <si>
+    <t>Súpergas</t>
+  </si>
+  <si>
+    <t>$ por kilo</t>
   </si>
 </sst>
 </file>
@@ -516,25 +588,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" customWidth="1"/>
-    <col min="5" max="5" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,367 +610,696 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="str">
+        <f>+J2</f>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J19" si="0">+J3</f>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6">
-        <f>+I5</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7">
-        <f>+I6</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8">
-        <f>+I7</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9">
-        <f>+I8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10">
-        <f>+I9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11">
-        <f>+I10</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="K14" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="K16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="K17" t="s">
         <v>43</v>
       </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" t="s">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="I13">
-        <v>1</v>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="K18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ActualizaciÃ³n completa: nuevas funcionalidades de cotizaciones, tipos de cambio multi-paÃ­s y mejoras en el sistema
</commit_message>
<xml_diff>
--- a/maestro_completo.xlsx
+++ b/maestro_completo.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jforrisi\Desktop\desarrollos\gita\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21468" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="maestro" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="76">
   <si>
     <t>id</t>
   </si>
@@ -45,121 +45,190 @@
     <t>activo</t>
   </si>
   <si>
-    <t>link</t>
+    <t>moneda</t>
+  </si>
+  <si>
+    <t>nominal_real</t>
+  </si>
+  <si>
+    <t>es_cotizacion</t>
+  </si>
+  <si>
+    <t>Precio hacienda</t>
+  </si>
+  <si>
+    <t>Leche en polvo</t>
+  </si>
+  <si>
+    <t>Queso</t>
+  </si>
+  <si>
+    <t>Precio leche productor</t>
+  </si>
+  <si>
+    <t>Precio carne export</t>
+  </si>
+  <si>
+    <t>Tipo de cambio USD/UYU (promedio compra-venta)</t>
+  </si>
+  <si>
+    <t>Tipo de cambio EUR/UYU (promedio compra-venta)</t>
+  </si>
+  <si>
+    <t>Soja</t>
+  </si>
+  <si>
+    <t>Arroz</t>
+  </si>
+  <si>
+    <t>Trigo</t>
+  </si>
+  <si>
+    <t>IPC</t>
+  </si>
+  <si>
+    <t>Celulosa -indice-</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Ingeniería</t>
+  </si>
+  <si>
+    <t>Arquitectura</t>
+  </si>
+  <si>
+    <t>Contabilidad (CPA)</t>
+  </si>
+  <si>
+    <t>Bookkeeping / payroll</t>
+  </si>
+  <si>
+    <t>Servicios no tradicionales - sin software</t>
+  </si>
+  <si>
+    <t>Salario real</t>
+  </si>
+  <si>
+    <t>Gasoil</t>
+  </si>
+  <si>
+    <t>Tipo de cambio USD/ARS (Argentina - Dólar CCL)</t>
+  </si>
+  <si>
+    <t>Tipo de cambio USD/BRL (Brasil)</t>
+  </si>
+  <si>
+    <t>Tipo de cambio USD/PEN (Perú - TC Interbancario Venta)</t>
+  </si>
+  <si>
+    <t>Tipo de cambio USD/CLP (Chile - Dólar Observado)</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>INAC – serie mensual precios de hacienda</t>
   </si>
   <si>
-    <t>M</t>
+    <t>INALE – Exportación leche en polvo entera</t>
+  </si>
+  <si>
+    <t>INALE – Exportación queso</t>
+  </si>
+  <si>
+    <t>INALE – Precio leche en tambo y composición</t>
+  </si>
+  <si>
+    <t>INE</t>
+  </si>
+  <si>
+    <t>WorldBank_CMO</t>
+  </si>
+  <si>
+    <t>INSEE - serie 010600341 (Producer Price Index - Pulp)</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>ANCAP</t>
+  </si>
+  <si>
+    <t>Rava_Scraping</t>
+  </si>
+  <si>
+    <t>BCB_API_PTAX</t>
+  </si>
+  <si>
+    <t>BCRP_API</t>
+  </si>
+  <si>
+    <t>BCCH_API</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>USD/kg</t>
   </si>
   <si>
+    <t>USD/ton</t>
+  </si>
+  <si>
+    <t>UYU/litro</t>
+  </si>
+  <si>
+    <t>UYU por USD</t>
+  </si>
+  <si>
+    <t>UYU por EUR</t>
+  </si>
+  <si>
+    <t>Indice</t>
+  </si>
+  <si>
+    <t>$ por Litro</t>
+  </si>
+  <si>
+    <t>ARS por USD</t>
+  </si>
+  <si>
+    <t>BRL por USD</t>
+  </si>
+  <si>
+    <t>PEN por USD</t>
+  </si>
+  <si>
+    <t>CLP por USD</t>
+  </si>
+  <si>
     <t>Carne</t>
   </si>
   <si>
-    <t>INALE – Exportación leche en polvo entera</t>
-  </si>
-  <si>
-    <t>USD/ton</t>
-  </si>
-  <si>
     <t>Lácteos</t>
   </si>
   <si>
-    <t>INALE – Exportación queso</t>
-  </si>
-  <si>
-    <t>INALE – Precio leche en tambo y composición</t>
-  </si>
-  <si>
-    <t>UYU/litro</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Tipo de cambio USD/UYU (promedio compra-venta)</t>
-  </si>
-  <si>
-    <t>INE</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>UYU por USD</t>
-  </si>
-  <si>
     <t>Macro</t>
   </si>
   <si>
-    <t>Tipo de cambio EUR/UYU (promedio compra-venta)</t>
-  </si>
-  <si>
-    <t>UYU por EUR</t>
-  </si>
-  <si>
-    <t>WorldBank_CMO</t>
-  </si>
-  <si>
     <t>Granos</t>
   </si>
   <si>
-    <t>IPC</t>
-  </si>
-  <si>
-    <t>Indice</t>
-  </si>
-  <si>
-    <t>INSEE - serie 010600341 (Producer Price Index - Pulp)</t>
-  </si>
-  <si>
     <t>Productos forestales</t>
   </si>
   <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>BLS</t>
-  </si>
-  <si>
-    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU513210513210</t>
-  </si>
-  <si>
-    <t>Ingeniería</t>
-  </si>
-  <si>
-    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU541330541330</t>
-  </si>
-  <si>
-    <t>Arquitectura</t>
-  </si>
-  <si>
-    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU541310541310</t>
-  </si>
-  <si>
-    <t>Contabilidad (CPA)</t>
-  </si>
-  <si>
-    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU541211541211</t>
-  </si>
-  <si>
-    <t>Bookkeeping / payroll</t>
-  </si>
-  <si>
-    <t>https://data.bls.gov/dataViewer/view/timeseries/PCU541211541211A</t>
-  </si>
-  <si>
-    <t>moneda</t>
+    <t>Macro - Tipo de cambio</t>
   </si>
   <si>
     <t>usd</t>
@@ -168,37 +237,7 @@
     <t>eur</t>
   </si>
   <si>
-    <t>Precio hacienda</t>
-  </si>
-  <si>
-    <t>Leche en polvo</t>
-  </si>
-  <si>
-    <t>Precio leche productor</t>
-  </si>
-  <si>
-    <t>Precio carne export</t>
-  </si>
-  <si>
-    <t>Soja</t>
-  </si>
-  <si>
-    <t>Arroz</t>
-  </si>
-  <si>
-    <t>Trigo</t>
-  </si>
-  <si>
-    <t>Celulosa -indice-</t>
-  </si>
-  <si>
-    <t>Servicios no tradicionales - sin software</t>
-  </si>
-  <si>
-    <t>Queso</t>
-  </si>
-  <si>
-    <t>nominal_real</t>
+    <t>uyu</t>
   </si>
   <si>
     <t>n</t>
@@ -207,25 +246,7 @@
     <t>r</t>
   </si>
   <si>
-    <t>Salario real</t>
-  </si>
-  <si>
-    <t>uyu</t>
-  </si>
-  <si>
-    <t>Gasoil</t>
-  </si>
-  <si>
-    <t>ANCAP</t>
-  </si>
-  <si>
-    <t>$ por Litro</t>
-  </si>
-  <si>
-    <t>Súpergas</t>
-  </si>
-  <si>
-    <t>$ por kilo</t>
+    <t>Servicios</t>
   </si>
 </sst>
 </file>
@@ -243,7 +264,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -304,7 +328,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -346,7 +370,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,9 +402,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,6 +437,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -588,16 +614,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="43.77734375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -625,13 +648,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -639,31 +662,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>73</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -671,32 +697,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" t="str">
-        <f>+J2</f>
-        <v>n</v>
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -704,32 +732,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" ref="J4:J19" si="0">+J3</f>
-        <v>n</v>
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -737,32 +767,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
+        <v>70</v>
+      </c>
+      <c r="J5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -770,32 +802,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
+        <v>70</v>
+      </c>
+      <c r="J6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -803,29 +837,32 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="0"/>
+        <f>+J6</f>
         <v>n</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -833,29 +870,32 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
+        <f>+J7</f>
         <v>n</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -863,32 +903,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
+        <v>70</v>
+      </c>
+      <c r="J9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -896,32 +938,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
-      </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
+        <v>70</v>
+      </c>
+      <c r="J10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -929,32 +973,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
+        <v>70</v>
+      </c>
+      <c r="J11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -962,29 +1008,32 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="0"/>
+        <f>+J11</f>
         <v>n</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -992,32 +1041,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>48</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
+        <v>71</v>
+      </c>
+      <c r="J13" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1025,32 +1076,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
-      </c>
-      <c r="K14" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="J14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1058,32 +1111,35 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>58</v>
+      </c>
+      <c r="G15" t="str">
+        <f>+G14</f>
+        <v>Servicios</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
-      </c>
-      <c r="K15" t="s">
-        <v>39</v>
+        <v>70</v>
+      </c>
+      <c r="J15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1091,32 +1147,35 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>58</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ref="G16:G21" si="0">+G15</f>
+        <v>Servicios</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
-      </c>
-      <c r="K16" t="s">
-        <v>41</v>
+        <v>70</v>
+      </c>
+      <c r="J16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1124,32 +1183,35 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>58</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>Servicios</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
-      </c>
-      <c r="K17" t="s">
-        <v>43</v>
+        <v>70</v>
+      </c>
+      <c r="J17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1157,32 +1219,35 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>58</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>Servicios</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
-      </c>
-      <c r="K18" t="s">
-        <v>45</v>
+        <v>70</v>
+      </c>
+      <c r="J18" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1190,29 +1255,35 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>58</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>Servicios</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="0"/>
-        <v>n</v>
+        <v>70</v>
+      </c>
+      <c r="J19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1220,28 +1291,35 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>58</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>Servicios</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="J20" t="s">
-        <v>61</v>
+        <v>74</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1249,60 +1327,178 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>Servicios</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="J21" t="s">
-        <v>60</v>
+        <v>73</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="G22" t="s">
+        <v>69</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" t="s">
+        <v>73</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" t="s">
+        <v>73</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
         <v>63</v>
       </c>
-      <c r="J22" t="s">
-        <v>60</v>
+      <c r="G25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" t="s">
+        <v>73</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>